<commit_message>
Finance Screen 50% Done
</commit_message>
<xml_diff>
--- a/Assets/Documentation/Asset List.xlsx
+++ b/Assets/Documentation/Asset List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-240" windowWidth="24915" windowHeight="12075" activeTab="4"/>
+    <workbookView xWindow="25005" yWindow="-150" windowWidth="28710" windowHeight="13395"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="237">
   <si>
     <t>Model Asset List</t>
   </si>
@@ -492,9 +492,6 @@
     <t xml:space="preserve">This is an idea to make it so the user can instantly build a completed room with no issues </t>
   </si>
   <si>
-    <t xml:space="preserve">Tabbed Build Menus </t>
-  </si>
-  <si>
     <t>Existing Properties</t>
   </si>
   <si>
@@ -724,6 +721,15 @@
   </si>
   <si>
     <t>Animated GUI</t>
+  </si>
+  <si>
+    <t>Video Analysis</t>
+  </si>
+  <si>
+    <t>Tabbed Menus</t>
+  </si>
+  <si>
+    <t>Radiator</t>
   </si>
 </sst>
 </file>
@@ -1154,10 +1160,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A3:I104"/>
+  <dimension ref="A3:I107"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B47" sqref="B46:B47"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,8 +1417,8 @@
       <c r="B29" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -1462,8 +1468,8 @@
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>27</v>
+      <c r="B35" s="6" t="s">
+        <v>236</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -1471,7 +1477,7 @@
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -1479,7 +1485,7 @@
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -1487,7 +1493,7 @@
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -1495,7 +1501,7 @@
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -1503,43 +1509,43 @@
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>84</v>
-      </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>97</v>
       </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="12" t="s">
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -1547,7 +1553,7 @@
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
@@ -1555,57 +1561,57 @@
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>34</v>
-      </c>
-      <c r="C47" s="5"/>
+      <c r="B47" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" s="4"/>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="12" t="s">
+      <c r="B48" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>13</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>12</v>
+      </c>
       <c r="B51" s="6" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
@@ -1613,133 +1619,133 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B52" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C52" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B53" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C53" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="C53" s="3"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>34</v>
-      </c>
       <c r="B54" s="6" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="12" t="s">
+      <c r="A55">
+        <v>34</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B57" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B58" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B59" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C59" s="5"/>
+        <v>63</v>
+      </c>
+      <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B60" s="7" t="s">
-        <v>66</v>
+        <v>234</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="12"/>
-      <c r="I61" s="12"/>
+      <c r="B61" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" s="5"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C62" s="5"/>
+      <c r="B62" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B63" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" t="s">
-        <v>148</v>
-      </c>
+      <c r="B63" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B64" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C64" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="C64" s="5"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
@@ -1747,7 +1753,7 @@
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="6" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
@@ -1755,7 +1761,7 @@
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -1763,50 +1769,47 @@
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C69" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="C69" s="4"/>
       <c r="D69" s="4"/>
-      <c r="E69" s="5"/>
+      <c r="E69" s="4"/>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C70" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="C70" s="4"/>
       <c r="D70" s="4"/>
-      <c r="E70" s="5"/>
+      <c r="E70" s="4"/>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C71" s="4"/>
+        <v>57</v>
+      </c>
+      <c r="C71" s="5"/>
       <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
+      <c r="E71" s="5"/>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C72" s="4"/>
+        <v>58</v>
+      </c>
+      <c r="C72" s="5"/>
       <c r="D72" s="4"/>
-      <c r="E72" s="4"/>
+      <c r="E72" s="5"/>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B73" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" t="s">
-        <v>148</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B74" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
@@ -1814,15 +1817,18 @@
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B75" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
+        <v>69</v>
+      </c>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B76" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
@@ -1830,7 +1836,7 @@
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B77" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
@@ -1838,7 +1844,7 @@
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="6" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
@@ -1846,7 +1852,7 @@
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79" s="6" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
@@ -1854,7 +1860,7 @@
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B80" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
@@ -1862,7 +1868,7 @@
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
@@ -1870,71 +1876,67 @@
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="6" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B83" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C83" s="12"/>
-      <c r="D83" s="12"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="12"/>
-      <c r="G83" s="12"/>
-      <c r="H83" s="12"/>
-      <c r="I83" s="12"/>
+      <c r="B83" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B84" s="7" t="s">
-        <v>52</v>
+      <c r="B84" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B85" s="7" t="s">
-        <v>53</v>
+      <c r="B85" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B86" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
+      <c r="B86" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C86" s="12"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="12"/>
+      <c r="G86" s="12"/>
+      <c r="H86" s="12"/>
+      <c r="I86" s="12"/>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B88" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C88" s="12"/>
-      <c r="D88" s="12"/>
-      <c r="E88" s="12"/>
-      <c r="F88" s="12"/>
-      <c r="G88" s="12"/>
-      <c r="H88" s="12"/>
-      <c r="I88" s="12"/>
+      <c r="B88" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="7" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
@@ -1942,43 +1944,43 @@
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="7" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B91" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C91" s="4"/>
-      <c r="D91" s="4"/>
-      <c r="E91" s="4"/>
+      <c r="B91" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C91" s="12"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="12"/>
+      <c r="H91" s="12"/>
+      <c r="I91" s="12"/>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B93" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C93" s="12"/>
-      <c r="D93" s="12"/>
-      <c r="E93" s="12"/>
-      <c r="F93" s="12"/>
-      <c r="G93" s="12"/>
-      <c r="H93" s="12"/>
-      <c r="I93" s="12"/>
+      <c r="B93" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="7" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
@@ -1986,23 +1988,27 @@
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="7" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B96" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C96" s="4"/>
-      <c r="D96" s="4"/>
-      <c r="E96" s="4"/>
+      <c r="B96" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C96" s="12"/>
+      <c r="D96" s="12"/>
+      <c r="E96" s="12"/>
+      <c r="F96" s="12"/>
+      <c r="G96" s="12"/>
+      <c r="H96" s="12"/>
+      <c r="I96" s="12"/>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="7" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
@@ -2010,27 +2016,23 @@
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="7" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B99" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="C99" s="12"/>
-      <c r="D99" s="12"/>
-      <c r="E99" s="12"/>
-      <c r="F99" s="12"/>
-      <c r="G99" s="12"/>
-      <c r="H99" s="12"/>
-      <c r="I99" s="12"/>
+      <c r="B99" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4"/>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
@@ -2038,23 +2040,27 @@
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B102" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C102" s="4"/>
-      <c r="D102" s="4"/>
-      <c r="E102" s="4"/>
+      <c r="B102" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C102" s="12"/>
+      <c r="D102" s="12"/>
+      <c r="E102" s="12"/>
+      <c r="F102" s="12"/>
+      <c r="G102" s="12"/>
+      <c r="H102" s="12"/>
+      <c r="I102" s="12"/>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
@@ -2062,23 +2068,47 @@
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
       <c r="E104" s="4"/>
     </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B105" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="4"/>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B106" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="4"/>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B107" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B83:I83"/>
-    <mergeCell ref="B88:I88"/>
-    <mergeCell ref="B93:I93"/>
-    <mergeCell ref="B99:I99"/>
+    <mergeCell ref="B86:I86"/>
+    <mergeCell ref="B91:I91"/>
+    <mergeCell ref="B96:I96"/>
+    <mergeCell ref="B102:I102"/>
     <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B42:I42"/>
-    <mergeCell ref="B48:I48"/>
-    <mergeCell ref="B55:I55"/>
-    <mergeCell ref="B61:I61"/>
+    <mergeCell ref="B43:I43"/>
+    <mergeCell ref="B49:I49"/>
+    <mergeCell ref="B56:I56"/>
+    <mergeCell ref="B63:I63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2456,8 +2486,8 @@
   </sheetPr>
   <dimension ref="B2:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D16:D17"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2521,208 +2551,208 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>157</v>
-      </c>
-      <c r="C12" s="4"/>
+        <v>235</v>
+      </c>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" t="s">
         <v>168</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C21" s="4"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>171</v>
-      </c>
-      <c r="C22" s="3"/>
+        <v>170</v>
+      </c>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C24" s="4"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C25" s="4"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C26" s="4"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C27" s="4"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C28" s="4"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C29" s="4"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C30" s="4"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C35" s="4"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C37" s="4"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C38" s="4"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C39" s="4"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C40" s="5"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C41" s="4"/>
     </row>
@@ -2734,76 +2764,76 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C44" s="4"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C45" s="5"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>199</v>
-      </c>
-      <c r="C46" s="4"/>
+        <v>198</v>
+      </c>
+      <c r="C46" s="5"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C47" s="4"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C48" s="4"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C49" s="4"/>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C50" s="4"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C51" s="5"/>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C52" s="4"/>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>233</v>
-      </c>
-      <c r="C53" s="4"/>
+        <v>232</v>
+      </c>
+      <c r="C53" s="3"/>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C54" s="3"/>
     </row>
@@ -2891,161 +2921,161 @@
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C16" s="11"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C23" s="3"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C24" s="3"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C25" s="4"/>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C27" s="5"/>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C28" s="5"/>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C30" s="5"/>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C31" s="5"/>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C33" s="5"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C34" s="5"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C35" s="5"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C36" s="5"/>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C38" s="3"/>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C39" s="3"/>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C40" s="3"/>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C41" s="5"/>
     </row>

</xml_diff>